<commit_message>
Added more experiment results
</commit_message>
<xml_diff>
--- a/Haskell/Grime Dice Real World Experiment.xlsx
+++ b/Haskell/Grime Dice Real World Experiment.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Creative\Nux-Git\Public Repos\proofs-grime-dice\Haskell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA40BC5A-D1B3-474F-8B79-88D271BD6ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A8003D-6226-431E-BF44-66B69AD6C187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38420" windowHeight="21000" xr2:uid="{BBD02365-F365-4EEB-9755-32219A4B15E7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38420" windowHeight="21000" activeTab="1" xr2:uid="{BBD02365-F365-4EEB-9755-32219A4B15E7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>red</t>
   </si>
@@ -204,7 +205,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$5</c:f>
+              <c:f>'Sheet1 (2)'!$A$1:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -227,7 +228,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$5</c:f>
+              <c:f>'Sheet1 (2)'!$B$1:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -251,7 +252,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4935-4995-9F45-C2C618020CC6}"/>
+              <c16:uniqueId val="{00000000-E287-4A25-B0C1-B6B70EE092A8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -532,7 +533,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$5</c:f>
+              <c:f>'Sheet1 (2)'!$A$1:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -555,7 +556,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$5</c:f>
+              <c:f>'Sheet1 (2)'!$C$1:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -579,7 +580,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EB75-4408-9E2B-9E8963CD1CD1}"/>
+              <c16:uniqueId val="{00000000-8129-4621-A198-9FA3540D8B02}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -757,6 +758,620 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Theoretical Limit</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>red</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>yellow</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>green</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.25925925925925902</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27777777777777701</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0.46296296296296202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4935-4995-9F45-C2C618020CC6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1171329503"/>
+        <c:axId val="1171326623"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1171329503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1171326623"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1171326623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.8"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1171329503"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Proportion Of Games WonOrTied So Far</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>red</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>yellow</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>green</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-182F-477B-A038-88F22F39534E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="158524704"/>
+        <c:axId val="158545824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="158524704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="158545824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="158545824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="158524704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -837,6 +1452,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1341,6 +2036,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1856,6 +3557,87 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>192181</xdr:colOff>
       <xdr:row>38</xdr:row>
+      <xdr:rowOff>138580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F4ADE60-0D27-471D-9D36-ADB143D30198}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>515471</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>186765</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>176306</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B72864D4-551A-4244-9357-B157DD40C0F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>496981</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>157630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>192181</xdr:colOff>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>138580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1884,22 +3666,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>515471</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>47812</xdr:rowOff>
+      <xdr:colOff>497051</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>80141</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>186765</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>176306</xdr:rowOff>
+      <xdr:colOff>199258</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>64375</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F222577F-71E6-9BF5-2CC8-2623C0787109}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03D3C878-70DE-2745-8EAD-714AE2511765}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2236,12 +4018,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E83B307-B148-48F5-BD3C-2A56C635C5B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF8A488-47F5-4DA3-B641-7C401BE3692C}">
   <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S9" sqref="R9:S9"/>
+      <selection pane="topRight" sqref="A1:T49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2471,4 +4253,160 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E83B307-B148-48F5-BD3C-2A56C635C5B1}">
+  <dimension ref="A1:AE4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T11" sqref="T11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0.25925925925925902</v>
+      </c>
+      <c r="C1">
+        <f>D1/$D$4</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D1" s="1">
+        <f>SUM(E1:BB1)</f>
+        <v>6</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="T1">
+        <v>1</v>
+      </c>
+      <c r="W1">
+        <v>1</v>
+      </c>
+      <c r="X1">
+        <v>1</v>
+      </c>
+      <c r="AB1">
+        <v>1</v>
+      </c>
+      <c r="AE1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.27777777777777701</v>
+      </c>
+      <c r="C2">
+        <f>D2/$D$4</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D3" si="0">SUM(E2:BB2)</f>
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.46296296296296202</v>
+      </c>
+      <c r="C3">
+        <f>D3/$D$4</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="D4" s="1">
+        <f>SUM(D1:D3)</f>
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>